<commit_message>
Ya se puede llenar la tabla PlatillosTeru de la base de datos con un csv, estos mismos también pueden ser usados en las comandas.
</commit_message>
<xml_diff>
--- a/Lista Platillos.xlsx
+++ b/Lista Platillos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documentos\Trabajo\TeruSistema\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
   <si>
     <t>Takoyaki</t>
   </si>
@@ -190,6 +195,21 @@
   </si>
   <si>
     <t>Bebida</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Platillo</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Plugin</t>
   </si>
 </sst>
 </file>
@@ -236,6 +256,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -284,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,7 +342,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,20 +562,23 @@
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -560,241 +586,307 @@
       <c r="C2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>55</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>65</v>
       </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>70</v>
       </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>45</v>
       </c>
       <c r="C18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>50</v>
@@ -802,10 +894,13 @@
       <c r="C24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>50</v>
@@ -813,10 +908,13 @@
       <c r="C25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>50</v>
@@ -824,21 +922,27 @@
       <c r="C26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>55</v>
@@ -846,10 +950,13 @@
       <c r="C28" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>55</v>
@@ -857,10 +964,13 @@
       <c r="C29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>55</v>
@@ -868,10 +978,13 @@
       <c r="C30" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>55</v>
@@ -879,21 +992,27 @@
       <c r="C31" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B32">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>60</v>
@@ -901,21 +1020,27 @@
       <c r="C33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>33</v>
-      </c>
-      <c r="B34">
-        <v>20</v>
-      </c>
-      <c r="C34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
       </c>
       <c r="B35">
         <v>20</v>
@@ -923,43 +1048,55 @@
       <c r="C35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>30</v>
       </c>
-      <c r="C36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>37</v>
-      </c>
-      <c r="B38">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
       </c>
       <c r="B39">
         <v>40</v>
@@ -967,131 +1104,167 @@
       <c r="C39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>30</v>
       </c>
-      <c r="C40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>30</v>
       </c>
-      <c r="C42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>40</v>
       </c>
-      <c r="C43" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>35</v>
       </c>
-      <c r="C45" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>40</v>
       </c>
-      <c r="C46" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>45</v>
       </c>
-      <c r="C47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>50</v>
       </c>
-      <c r="C48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>45</v>
       </c>
-      <c r="C49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C50" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>49</v>
-      </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
       </c>
       <c r="B51">
         <v>10</v>
@@ -1099,10 +1272,13 @@
       <c r="C51" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>10</v>
@@ -1110,31 +1286,55 @@
       <c r="C52" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>20</v>
       </c>
-      <c r="C53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C54" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>10</v>
       </c>
-      <c r="C54" t="s">
-        <v>57</v>
+      <c r="C55" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>